<commit_message>
menos neuro mais erro '
</commit_message>
<xml_diff>
--- a/nuno-dataset/test-solidos-02/content/results/metrics_14_5.xlsx
+++ b/nuno-dataset/test-solidos-02/content/results/metrics_14_5.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,63 +478,63 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>model_14_5_1</t>
+          <t>model_14_5_0</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7188192439008758</v>
+        <v>0.5010782282294184</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5665314748195951</v>
+        <v>0.3791495606328492</v>
       </c>
       <c r="D2" t="n">
-        <v>0.7758671181154178</v>
+        <v>0.3917534915799327</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6899480985482878</v>
+        <v>0.4477410905295015</v>
       </c>
       <c r="F2" t="n">
-        <v>33.91048431396484</v>
+        <v>60.17011260986328</v>
       </c>
       <c r="G2" t="n">
-        <v>61.40763854980469</v>
+        <v>94.49362182617188</v>
       </c>
       <c r="H2" t="n">
-        <v>38.24813079833984</v>
+        <v>36.31206130981445</v>
       </c>
       <c r="I2" t="n">
-        <v>50.50904846191406</v>
+        <v>67.11407470703125</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>model_14_5_0</t>
+          <t>model_14_5_1</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.7216158346792649</v>
+        <v>0.5122750834436902</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6126909889820396</v>
+        <v>0.3583494960628629</v>
       </c>
       <c r="D3" t="n">
-        <v>0.8093793205550223</v>
+        <v>0.4237981594061286</v>
       </c>
       <c r="E3" t="n">
-        <v>0.7277195961881784</v>
+        <v>0.4413578063043367</v>
       </c>
       <c r="F3" t="n">
-        <v>33.57321166992188</v>
+        <v>58.81977081298828</v>
       </c>
       <c r="G3" t="n">
-        <v>54.86841583251953</v>
+        <v>97.65940093994141</v>
       </c>
       <c r="H3" t="n">
-        <v>32.529296875</v>
+        <v>34.39900588989258</v>
       </c>
       <c r="I3" t="n">
-        <v>44.35587310791016</v>
+        <v>67.88980865478516</v>
       </c>
     </row>
     <row r="4">
@@ -544,28 +544,28 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.7234679775972048</v>
+        <v>0.5317061992022282</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4598319778923317</v>
+        <v>0.4122970122918594</v>
       </c>
       <c r="D4" t="n">
-        <v>0.7597519547264865</v>
+        <v>0.3899932546234153</v>
       </c>
       <c r="E4" t="n">
-        <v>0.6328808424792056</v>
+        <v>0.4693121976685155</v>
       </c>
       <c r="F4" t="n">
-        <v>33.34984588623047</v>
+        <v>56.47637176513672</v>
       </c>
       <c r="G4" t="n">
-        <v>76.52330017089844</v>
+        <v>89.44857025146484</v>
       </c>
       <c r="H4" t="n">
-        <v>40.99817276000977</v>
+        <v>36.41714477539062</v>
       </c>
       <c r="I4" t="n">
-        <v>59.80559158325195</v>
+        <v>64.49261474609375</v>
       </c>
     </row>
     <row r="5">
@@ -575,28 +575,28 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.7526359107888241</v>
+        <v>0.5404194849343491</v>
       </c>
       <c r="C5" t="n">
-        <v>0.5348271786956076</v>
+        <v>0.3501516123105428</v>
       </c>
       <c r="D5" t="n">
-        <v>0.7470854984428827</v>
+        <v>0.4718104776777189</v>
       </c>
       <c r="E5" t="n">
-        <v>0.6611636774951962</v>
+        <v>0.4470216793759235</v>
       </c>
       <c r="F5" t="n">
-        <v>29.83218383789062</v>
+        <v>55.42554473876953</v>
       </c>
       <c r="G5" t="n">
-        <v>65.89905548095703</v>
+        <v>98.90712738037109</v>
       </c>
       <c r="H5" t="n">
-        <v>43.15969467163086</v>
+        <v>31.53269195556641</v>
       </c>
       <c r="I5" t="n">
-        <v>55.19817352294922</v>
+        <v>67.20149993896484</v>
       </c>
     </row>
     <row r="6">
@@ -606,121 +606,121 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.7575841138077719</v>
+        <v>0.5410780975414631</v>
       </c>
       <c r="C6" t="n">
-        <v>0.4663022982396277</v>
+        <v>0.3005365506773902</v>
       </c>
       <c r="D6" t="n">
-        <v>0.7444011328736277</v>
+        <v>0.4661037619969374</v>
       </c>
       <c r="E6" t="n">
-        <v>0.6282924003410246</v>
+        <v>0.4128056336692332</v>
       </c>
       <c r="F6" t="n">
-        <v>29.23542785644531</v>
+        <v>55.34611129760742</v>
       </c>
       <c r="G6" t="n">
-        <v>75.60668182373047</v>
+        <v>106.4585494995117</v>
       </c>
       <c r="H6" t="n">
-        <v>43.61777877807617</v>
+        <v>31.87338066101074</v>
       </c>
       <c r="I6" t="n">
-        <v>60.55307769775391</v>
+        <v>71.35964965820312</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>model_14_5_6</t>
+          <t>model_14_5_5</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.7684996735102603</v>
+        <v>0.5717831119780701</v>
       </c>
       <c r="C7" t="n">
-        <v>0.4285630700220719</v>
+        <v>0.3574807712641276</v>
       </c>
       <c r="D7" t="n">
-        <v>0.7326629457130962</v>
+        <v>0.5401807992196365</v>
       </c>
       <c r="E7" t="n">
-        <v>0.6051312181445232</v>
+        <v>0.4676866370233626</v>
       </c>
       <c r="F7" t="n">
-        <v>27.91900825500488</v>
+        <v>51.64308547973633</v>
       </c>
       <c r="G7" t="n">
-        <v>80.95303344726562</v>
+        <v>97.7916259765625</v>
       </c>
       <c r="H7" t="n">
-        <v>45.62089538574219</v>
+        <v>27.45101165771484</v>
       </c>
       <c r="I7" t="n">
-        <v>64.32614898681641</v>
+        <v>64.69015502929688</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>model_14_5_5</t>
+          <t>model_14_5_11</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.7704571756280686</v>
+        <v>0.5723071582572985</v>
       </c>
       <c r="C8" t="n">
-        <v>0.474431173880703</v>
+        <v>0.3078130582154748</v>
       </c>
       <c r="D8" t="n">
-        <v>0.7483886158846897</v>
+        <v>0.1544761545927709</v>
       </c>
       <c r="E8" t="n">
-        <v>0.6340003993584564</v>
+        <v>0.3455896828925454</v>
       </c>
       <c r="F8" t="n">
-        <v>27.68293190002441</v>
+        <v>51.57988357543945</v>
       </c>
       <c r="G8" t="n">
-        <v>74.45509338378906</v>
+        <v>105.3510589599609</v>
       </c>
       <c r="H8" t="n">
-        <v>42.93731689453125</v>
+        <v>50.4774169921875</v>
       </c>
       <c r="I8" t="n">
-        <v>59.62321472167969</v>
+        <v>79.52816772460938</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>model_14_5_7</t>
+          <t>model_14_5_9</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.7722166036937503</v>
+        <v>0.5823706731643306</v>
       </c>
       <c r="C9" t="n">
-        <v>0.4088311356072766</v>
+        <v>0.3331708866462276</v>
       </c>
       <c r="D9" t="n">
-        <v>0.7188197538103283</v>
+        <v>0.3880416617807921</v>
       </c>
       <c r="E9" t="n">
-        <v>0.5892227943444696</v>
+        <v>0.4163974235730167</v>
       </c>
       <c r="F9" t="n">
-        <v>27.47074317932129</v>
+        <v>50.36621856689453</v>
       </c>
       <c r="G9" t="n">
-        <v>83.74837493896484</v>
+        <v>101.4915924072266</v>
       </c>
       <c r="H9" t="n">
-        <v>47.98322296142578</v>
+        <v>36.53365325927734</v>
       </c>
       <c r="I9" t="n">
-        <v>66.91771697998047</v>
+        <v>70.92315673828125</v>
       </c>
     </row>
     <row r="10">
@@ -730,462 +730,369 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.7820880988355638</v>
+        <v>0.5881247841330518</v>
       </c>
       <c r="C10" t="n">
-        <v>0.4299180728352087</v>
+        <v>0.3410415169206469</v>
       </c>
       <c r="D10" t="n">
-        <v>0.6949359057733493</v>
+        <v>0.4766023918389489</v>
       </c>
       <c r="E10" t="n">
-        <v>0.5871571571626681</v>
+        <v>0.442089009402578</v>
       </c>
       <c r="F10" t="n">
-        <v>26.28023910522461</v>
+        <v>49.67227554321289</v>
       </c>
       <c r="G10" t="n">
-        <v>80.76107788085938</v>
+        <v>100.2936859130859</v>
       </c>
       <c r="H10" t="n">
-        <v>52.05898666381836</v>
+        <v>31.24661636352539</v>
       </c>
       <c r="I10" t="n">
-        <v>67.25421142578125</v>
+        <v>67.80094146728516</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>model_14_5_9</t>
+          <t>model_14_5_7</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.7849273560535748</v>
+        <v>0.5886548588049501</v>
       </c>
       <c r="C11" t="n">
-        <v>0.42143929759103</v>
+        <v>0.3393866515743771</v>
       </c>
       <c r="D11" t="n">
-        <v>0.6863836637931482</v>
+        <v>0.4938428585284789</v>
       </c>
       <c r="E11" t="n">
-        <v>0.5790378269812004</v>
+        <v>0.4449773289099012</v>
       </c>
       <c r="F11" t="n">
-        <v>25.93782424926758</v>
+        <v>49.60834503173828</v>
       </c>
       <c r="G11" t="n">
-        <v>81.96223449707031</v>
+        <v>100.5455551147461</v>
       </c>
       <c r="H11" t="n">
-        <v>53.51842498779297</v>
+        <v>30.21736907958984</v>
       </c>
       <c r="I11" t="n">
-        <v>68.57689666748047</v>
+        <v>67.44994354248047</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>model_14_5_22</t>
+          <t>model_14_5_6</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.7871192185515063</v>
+        <v>0.5910898876767523</v>
       </c>
       <c r="C12" t="n">
-        <v>0.3732352104046813</v>
+        <v>0.3456349737453623</v>
       </c>
       <c r="D12" t="n">
-        <v>0.6430237927975164</v>
+        <v>0.5592085369645083</v>
       </c>
       <c r="E12" t="n">
-        <v>0.5354705409969531</v>
+        <v>0.464231152874453</v>
       </c>
       <c r="F12" t="n">
-        <v>25.67348289489746</v>
+        <v>49.31467819213867</v>
       </c>
       <c r="G12" t="n">
-        <v>88.79109191894531</v>
+        <v>99.59455871582031</v>
       </c>
       <c r="H12" t="n">
-        <v>60.91775512695312</v>
+        <v>26.31506538391113</v>
       </c>
       <c r="I12" t="n">
-        <v>75.67423248291016</v>
+        <v>65.11008453369141</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>model_14_5_21</t>
+          <t>model_14_5_18</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.7879561570013363</v>
+        <v>0.593398236751963</v>
       </c>
       <c r="C13" t="n">
-        <v>0.3771577554230655</v>
+        <v>0.2580415519884932</v>
       </c>
       <c r="D13" t="n">
-        <v>0.6438289684487419</v>
+        <v>0.4504085688605136</v>
       </c>
       <c r="E13" t="n">
-        <v>0.537673397975859</v>
+        <v>0.381001555309985</v>
       </c>
       <c r="F13" t="n">
-        <v>25.57254981994629</v>
+        <v>49.03629302978516</v>
       </c>
       <c r="G13" t="n">
-        <v>88.23540496826172</v>
+        <v>112.9263076782227</v>
       </c>
       <c r="H13" t="n">
-        <v>60.78035736083984</v>
+        <v>32.81037521362305</v>
       </c>
       <c r="I13" t="n">
-        <v>75.31536865234375</v>
+        <v>75.22468566894531</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>model_14_5_20</t>
+          <t>model_14_5_12</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.7889205318091564</v>
+        <v>0.5942031478790619</v>
       </c>
       <c r="C14" t="n">
-        <v>0.3841195382909653</v>
+        <v>0.2990034513669816</v>
       </c>
       <c r="D14" t="n">
-        <v>0.6447578324635511</v>
+        <v>0.430647170996982</v>
       </c>
       <c r="E14" t="n">
-        <v>0.5413363867777254</v>
+        <v>0.4035924742312659</v>
       </c>
       <c r="F14" t="n">
-        <v>25.45624923706055</v>
+        <v>48.9392204284668</v>
       </c>
       <c r="G14" t="n">
-        <v>87.24916076660156</v>
+        <v>106.6918869018555</v>
       </c>
       <c r="H14" t="n">
-        <v>60.62184143066406</v>
+        <v>33.99011993408203</v>
       </c>
       <c r="I14" t="n">
-        <v>74.71865844726562</v>
+        <v>72.47930145263672</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>model_14_5_19</t>
+          <t>model_14_5_16</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.7903474439790713</v>
+        <v>0.5945671373100367</v>
       </c>
       <c r="C15" t="n">
-        <v>0.3944160967622141</v>
+        <v>0.2706326728773504</v>
       </c>
       <c r="D15" t="n">
-        <v>0.6467230160030752</v>
+        <v>0.4462712844753584</v>
       </c>
       <c r="E15" t="n">
-        <v>0.5470455344634841</v>
+        <v>0.388393505802792</v>
       </c>
       <c r="F15" t="n">
-        <v>25.28416061401367</v>
+        <v>48.89532470703125</v>
       </c>
       <c r="G15" t="n">
-        <v>85.79049682617188</v>
+        <v>111.0099258422852</v>
       </c>
       <c r="H15" t="n">
-        <v>60.28648376464844</v>
+        <v>33.057373046875</v>
       </c>
       <c r="I15" t="n">
-        <v>73.78861236572266</v>
+        <v>74.32637023925781</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>model_14_5_18</t>
+          <t>model_14_5_17</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.7906625088001537</v>
+        <v>0.5960926295059297</v>
       </c>
       <c r="C16" t="n">
-        <v>0.397027494809812</v>
+        <v>0.2723927272675806</v>
       </c>
       <c r="D16" t="n">
-        <v>0.6469965126492243</v>
+        <v>0.4542532680141328</v>
       </c>
       <c r="E16" t="n">
-        <v>0.5483825932525763</v>
+        <v>0.3914057259748337</v>
       </c>
       <c r="F16" t="n">
-        <v>25.24616432189941</v>
+        <v>48.71135330200195</v>
       </c>
       <c r="G16" t="n">
-        <v>85.42054748535156</v>
+        <v>110.7420425415039</v>
       </c>
       <c r="H16" t="n">
-        <v>60.23981475830078</v>
+        <v>32.58084869384766</v>
       </c>
       <c r="I16" t="n">
-        <v>73.57079315185547</v>
+        <v>73.96030426025391</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>model_14_5_10</t>
+          <t>model_14_5_13</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.7909776258259271</v>
+        <v>0.5962891782073554</v>
       </c>
       <c r="C17" t="n">
-        <v>0.4349555093314732</v>
+        <v>0.3057080839644775</v>
       </c>
       <c r="D17" t="n">
-        <v>0.6747804025417153</v>
+        <v>0.4356218581596593</v>
       </c>
       <c r="E17" t="n">
-        <v>0.5795405364507769</v>
+        <v>0.4091878988010755</v>
       </c>
       <c r="F17" t="n">
-        <v>25.20816040039062</v>
+        <v>48.68764495849609</v>
       </c>
       <c r="G17" t="n">
-        <v>80.04744720458984</v>
+        <v>105.6714401245117</v>
       </c>
       <c r="H17" t="n">
-        <v>55.49851226806641</v>
+        <v>33.69313430786133</v>
       </c>
       <c r="I17" t="n">
-        <v>68.49500274658203</v>
+        <v>71.79930114746094</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>model_14_5_17</t>
+          <t>model_14_5_15</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.7917328975520058</v>
+        <v>0.5975831235476825</v>
       </c>
       <c r="C18" t="n">
-        <v>0.4085525486840363</v>
+        <v>0.2893974432227321</v>
       </c>
       <c r="D18" t="n">
-        <v>0.6530655525354701</v>
+        <v>0.4495798754731949</v>
       </c>
       <c r="E18" t="n">
-        <v>0.5566803899427601</v>
+        <v>0.4016001204619458</v>
       </c>
       <c r="F18" t="n">
-        <v>25.11707496643066</v>
+        <v>48.53159332275391</v>
       </c>
       <c r="G18" t="n">
-        <v>83.78783416748047</v>
+        <v>108.153923034668</v>
       </c>
       <c r="H18" t="n">
-        <v>59.20413589477539</v>
+        <v>32.85984802246094</v>
       </c>
       <c r="I18" t="n">
-        <v>72.21903991699219</v>
+        <v>72.72142028808594</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>model_14_5_12</t>
+          <t>model_14_5_10</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.7924749114419452</v>
+        <v>0.597704652195519</v>
       </c>
       <c r="C19" t="n">
-        <v>0.4250480315879348</v>
+        <v>0.3366048039421951</v>
       </c>
       <c r="D19" t="n">
-        <v>0.6610854657107283</v>
+        <v>0.4451673428492053</v>
       </c>
       <c r="E19" t="n">
-        <v>0.5682281144890153</v>
+        <v>0.4318802956374783</v>
       </c>
       <c r="F19" t="n">
-        <v>25.027587890625</v>
+        <v>48.51693725585938</v>
       </c>
       <c r="G19" t="n">
-        <v>81.45098876953125</v>
+        <v>100.9689559936523</v>
       </c>
       <c r="H19" t="n">
-        <v>57.83554458618164</v>
+        <v>33.12327575683594</v>
       </c>
       <c r="I19" t="n">
-        <v>70.33785247802734</v>
+        <v>69.04157257080078</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>model_14_5_11</t>
+          <t>model_14_5_14</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.7926035815570951</v>
+        <v>0.5997646965575385</v>
       </c>
       <c r="C20" t="n">
-        <v>0.4327968716939861</v>
+        <v>0.3116277826452079</v>
       </c>
       <c r="D20" t="n">
-        <v>0.6700305331880225</v>
+        <v>0.4522606734635393</v>
       </c>
       <c r="E20" t="n">
-        <v>0.5762051655466813</v>
+        <v>0.4169594158510636</v>
       </c>
       <c r="F20" t="n">
-        <v>25.0120677947998</v>
+        <v>48.26849365234375</v>
       </c>
       <c r="G20" t="n">
-        <v>80.35324859619141</v>
+        <v>104.7704696655273</v>
       </c>
       <c r="H20" t="n">
-        <v>56.30907440185547</v>
+        <v>32.69980621337891</v>
       </c>
       <c r="I20" t="n">
-        <v>69.03835296630859</v>
+        <v>70.8548583984375</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>model_14_5_16</t>
+          <t>model_14_5_19</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.7926851762345462</v>
+        <v>0.6002080052318077</v>
       </c>
       <c r="C21" t="n">
-        <v>0.4125075173457247</v>
+        <v>0.2788187579834575</v>
       </c>
       <c r="D21" t="n">
-        <v>0.6562808351878726</v>
+        <v>0.4762574281715917</v>
       </c>
       <c r="E21" t="n">
-        <v>0.5600862037542027</v>
+        <v>0.4007532291321236</v>
       </c>
       <c r="F21" t="n">
-        <v>25.00222969055176</v>
+        <v>48.21503067016602</v>
       </c>
       <c r="G21" t="n">
-        <v>83.22755432128906</v>
+        <v>109.7640075683594</v>
       </c>
       <c r="H21" t="n">
-        <v>58.65545272827148</v>
+        <v>31.26720809936523</v>
       </c>
       <c r="I21" t="n">
-        <v>71.66421508789062</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="inlineStr">
-        <is>
-          <t>model_14_5_15</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>0.7926857422892021</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0.4208282591181479</v>
-      </c>
-      <c r="D22" t="n">
-        <v>0.6596114599989675</v>
-      </c>
-      <c r="E22" t="n">
-        <v>0.5655588562216785</v>
-      </c>
-      <c r="F22" t="n">
-        <v>25.00216102600098</v>
-      </c>
-      <c r="G22" t="n">
-        <v>82.04879760742188</v>
-      </c>
-      <c r="H22" t="n">
-        <v>58.08708190917969</v>
-      </c>
-      <c r="I22" t="n">
-        <v>70.77268981933594</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="inlineStr">
-        <is>
-          <t>model_14_5_13</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>0.7933326582680003</v>
-      </c>
-      <c r="C23" t="n">
-        <v>0.4251372654216189</v>
-      </c>
-      <c r="D23" t="n">
-        <v>0.6617347785971694</v>
-      </c>
-      <c r="E23" t="n">
-        <v>0.5685893796917934</v>
-      </c>
-      <c r="F23" t="n">
-        <v>24.92414283752441</v>
-      </c>
-      <c r="G23" t="n">
-        <v>81.43834686279297</v>
-      </c>
-      <c r="H23" t="n">
-        <v>57.72473907470703</v>
-      </c>
-      <c r="I23" t="n">
-        <v>70.27899932861328</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="inlineStr">
-        <is>
-          <t>model_14_5_14</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>0.793455378695981</v>
-      </c>
-      <c r="C24" t="n">
-        <v>0.4244238555107573</v>
-      </c>
-      <c r="D24" t="n">
-        <v>0.6608014781599317</v>
-      </c>
-      <c r="E24" t="n">
-        <v>0.5678008674674568</v>
-      </c>
-      <c r="F24" t="n">
-        <v>24.90934371948242</v>
-      </c>
-      <c r="G24" t="n">
-        <v>81.53942108154297</v>
-      </c>
-      <c r="H24" t="n">
-        <v>57.88400268554688</v>
-      </c>
-      <c r="I24" t="n">
-        <v>70.40745544433594</v>
+        <v>72.8243408203125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>